<commit_message>
thu hồi sản phẩm đã xoá
</commit_message>
<xml_diff>
--- a/cn.xlsx
+++ b/cn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\PHP\quanlycuahang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650CE2F1-F413-42F4-BF01-474EF0B4CDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25320D1-224B-4B3F-99E0-34332B04AEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23040" yWindow="3000" windowWidth="18000" windowHeight="9750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -614,7 +614,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
@@ -622,12 +622,15 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>